<commit_message>
cleaned up the TSA Traffic section of the notebook and updated diagram and dictionary
</commit_message>
<xml_diff>
--- a/project3/air-travel-data-dict-v3.xlsx
+++ b/project3/air-travel-data-dict-v3.xlsx
@@ -14,14 +14,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="g7eQ8enMnkeGMBxEznHc2F3SIV9IyYYCfXxjUzZt6CU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="XnMWkl7AJc1vLpe2eOYFjFPLYp1fb3GtYJtPFgMOEy4="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="159">
   <si>
     <t>Origin Source</t>
   </si>
@@ -170,7 +170,7 @@
     <t>when this table was loaded into the lakehouse</t>
   </si>
   <si>
-    <t>Extraction Scripts</t>
+    <t>Data Pull Scripts</t>
   </si>
   <si>
     <t>N/A</t>
@@ -500,10 +500,10 @@
     <t>tsa_traffic</t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>hour</t>
+    <t>event_date</t>
+  </si>
+  <si>
+    <t>event_hour</t>
   </si>
   <si>
     <t>airport_code</t>
@@ -618,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -630,6 +630,9 @@
     </xf>
     <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
@@ -654,6 +657,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -662,6 +668,9 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1174,7 +1183,7 @@
       <c r="A30" s="3"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2332,130 +2341,130 @@
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7"/>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="7"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="7"/>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="7"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -2491,27 +2500,27 @@
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="8"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2544,29 +2553,29 @@
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2599,97 +2608,97 @@
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="7"/>
+      <c r="C51" s="8"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D52" s="7"/>
+      <c r="D52" s="8"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D53" s="7"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D54" s="7"/>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D55" s="7"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="7"/>
+      <c r="D56" s="8"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D57" s="7"/>
+      <c r="D57" s="8"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D58" s="7"/>
+      <c r="D58" s="8"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="11" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2717,7 +2726,7 @@
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3747,88 +3756,88 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -3861,7 +3870,7 @@
       <c r="A17" s="3"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4896,124 +4905,124 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="11"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="12"/>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
@@ -5038,47 +5047,47 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="14"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
     </row>
     <row r="20">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
     </row>
     <row r="21">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
     </row>
     <row r="22">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
     </row>
     <row r="23">
-      <c r="A23" s="13"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5102,266 +5111,288 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="11" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="11" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5400,8 +5431,8 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>57</v>
+      <c r="A4" s="20" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
@@ -5414,7 +5445,7 @@
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1"/>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>